<commit_message>
[tests] add new tests
</commit_message>
<xml_diff>
--- a/web/fixtures/csv/test_data/carbure_template_advanced_missing_data_cannot_validate.xlsx
+++ b/web/fixtures/csv/test_data/carbure_template_advanced_missing_data_cannot_validate.xlsx
@@ -25,7 +25,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="919">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="921">
+  <si>
+    <t xml:space="preserve">commentaire</t>
+  </si>
   <si>
     <t xml:space="preserve">producer</t>
   </si>
@@ -105,6 +108,9 @@
     <t xml:space="preserve">mac</t>
   </si>
   <si>
+    <t xml:space="preserve">pas de certificat</t>
+  </si>
+  <si>
     <t xml:space="preserve">TOTOPOUET</t>
   </si>
   <si>
@@ -114,9 +120,6 @@
     <t xml:space="preserve">FR</t>
   </si>
   <si>
-    <t xml:space="preserve">2004-06-01</t>
-  </si>
-  <si>
     <t xml:space="preserve">ETH</t>
   </si>
   <si>
@@ -139,6 +142,9 @@
   </si>
   <si>
     <t xml:space="preserve">529</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pas de date de mise en service</t>
   </si>
   <si>
     <t xml:space="preserve">ISCC-ES-100002010</t>
@@ -2788,8 +2794,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -2865,7 +2872,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2874,42 +2881,46 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z1048576"/>
+  <dimension ref="A1:AA3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="35.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="28.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="35.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.6"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -2987,25 +2998,28 @@
       <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="D2" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>38139</v>
+      </c>
+      <c r="H2" s="0" t="n">
         <v>35549</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>30</v>
       </c>
       <c r="I2" s="0" t="s">
         <v>31</v>
@@ -3013,23 +3027,23 @@
       <c r="J2" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="K2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="L2" s="0" t="n">
+      <c r="M2" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="M2" s="0" t="n">
+      <c r="N2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="N2" s="0" t="n">
+      <c r="O2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O2" s="0" t="n">
+      <c r="P2" s="0" t="n">
         <v>1.9</v>
-      </c>
-      <c r="P2" s="0" t="n">
-        <v>0</v>
       </c>
       <c r="Q2" s="0" t="n">
         <v>0</v>
@@ -3040,8 +3054,8 @@
       <c r="S2" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="T2" s="0" t="s">
-        <v>33</v>
+      <c r="T2" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="U2" s="0" t="s">
         <v>34</v>
@@ -3056,30 +3070,33 @@
         <v>37</v>
       </c>
       <c r="Y2" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z2" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="Z2" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA2" s="0" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="0" t="n">
         <v>35549</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>30</v>
       </c>
       <c r="I3" s="0" t="s">
         <v>31</v>
@@ -3087,23 +3104,23 @@
       <c r="J3" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="0" t="n">
+      <c r="K3" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="L3" s="0" t="n">
+      <c r="M3" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="M3" s="0" t="n">
+      <c r="N3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="N3" s="0" t="n">
+      <c r="O3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O3" s="0" t="n">
+      <c r="P3" s="0" t="n">
         <v>1.9</v>
-      </c>
-      <c r="P3" s="0" t="n">
-        <v>0</v>
       </c>
       <c r="Q3" s="0" t="n">
         <v>0</v>
@@ -3114,14 +3131,14 @@
       <c r="S3" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="T3" s="0" t="s">
-        <v>33</v>
+      <c r="T3" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="U3" s="0" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="V3" s="0" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="W3" s="0" t="s">
         <v>36</v>
@@ -3130,21 +3147,15 @@
         <v>37</v>
       </c>
       <c r="Y3" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z3" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="Z3" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA3" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -3157,7 +3168,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3167,305 +3178,302 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -3480,7 +3488,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3490,177 +3498,174 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -3675,7 +3680,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3685,2025 +3690,2022 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="B113" s="0" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B114" s="0" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="B115" s="0" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="B116" s="0" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="B117" s="0" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="B118" s="0" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="B119" s="0" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="B120" s="0" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B121" s="0" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="B122" s="0" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="B123" s="0" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="B124" s="0" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="B125" s="0" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="B126" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B127" s="0" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="B128" s="0" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B129" s="0" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="B130" s="0" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="B131" s="0" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="B132" s="0" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="B133" s="0" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="B134" s="0" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="B135" s="0" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="B136" s="0" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="B137" s="0" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="B138" s="0" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="B139" s="0" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="B140" s="0" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="B141" s="0" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="B142" s="0" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="B143" s="0" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="B144" s="0" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="B145" s="0" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="B146" s="0" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="B147" s="0" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="B148" s="0" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="B149" s="0" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="B150" s="0" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="B151" s="0" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="B152" s="0" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="B153" s="0" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="B154" s="0" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B155" s="0" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="B156" s="0" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="B157" s="0" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="B158" s="0" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="B159" s="0" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="B160" s="0" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="B161" s="0" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="B162" s="0" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="B163" s="0" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="B164" s="0" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="B165" s="0" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="B166" s="0" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="B167" s="0" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="B168" s="0" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="B169" s="0" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="B170" s="0" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="B171" s="0" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="B172" s="0" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="B173" s="0" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="B174" s="0" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="B175" s="0" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="B176" s="0" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="B177" s="0" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="B178" s="0" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="B179" s="0" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="B180" s="0" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="B181" s="0" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="B182" s="0" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="B183" s="0" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="B184" s="0" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="B185" s="0" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="B186" s="0" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="B187" s="0" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="B188" s="0" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="B189" s="0" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="B190" s="0" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="B191" s="0" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="B192" s="0" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="B193" s="0" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="B194" s="0" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="B195" s="0" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="B196" s="0" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="B197" s="0" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="B198" s="0" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="B199" s="0" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="B200" s="0" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="B201" s="0" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="B202" s="0" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="B203" s="0" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="B204" s="0" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="B205" s="0" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="B206" s="0" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="B207" s="0" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="B208" s="0" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="B209" s="0" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="B210" s="0" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="B211" s="0" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="B212" s="0" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="B213" s="0" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
     </row>
     <row r="214" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="B214" s="0" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="B215" s="0" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
     </row>
     <row r="216" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="B216" s="0" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
     </row>
     <row r="217" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="B217" s="0" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
     </row>
     <row r="218" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="B218" s="0" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="B219" s="0" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="B220" s="0" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="B221" s="0" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="B222" s="0" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
     </row>
     <row r="223" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="B223" s="0" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
     </row>
     <row r="224" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="B224" s="0" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
     </row>
     <row r="225" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="B225" s="0" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
     </row>
     <row r="226" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="B226" s="0" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="B227" s="0" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
     </row>
     <row r="228" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="B228" s="0" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="0" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="B229" s="0" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="0" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="B230" s="0" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="0" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="B231" s="0" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="B232" s="0" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="0" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="B233" s="0" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
     </row>
     <row r="234" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="0" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="B234" s="0" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
     </row>
     <row r="235" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="B235" s="0" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
     </row>
     <row r="236" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="0" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="B236" s="0" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
     </row>
     <row r="237" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="B237" s="0" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="0" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="B238" s="0" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="0" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="B239" s="0" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
     </row>
     <row r="240" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="0" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="B240" s="0" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="0" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="B241" s="0" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="B242" s="0" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="0" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="B243" s="0" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="0" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="B244" s="0" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
     </row>
     <row r="245" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="0" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="B245" s="0" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
     </row>
     <row r="246" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="0" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="B246" s="0" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
     </row>
     <row r="247" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="0" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="B247" s="0" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
     </row>
     <row r="248" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="0" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="B248" s="0" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
     </row>
     <row r="249" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="0" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="B249" s="0" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
     </row>
     <row r="250" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="0" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c r="B250" s="0" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
     </row>
     <row r="251" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="0" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="B251" s="0" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="0" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="B252" s="0" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
     </row>
   </sheetData>
@@ -5718,7 +5720,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -5728,279 +5730,276 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
     </row>
   </sheetData>
@@ -6015,7 +6014,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -6025,897 +6024,894 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="B15" s="0" t="s">
+        <v>733</v>
+      </c>
+      <c r="C15" s="0" t="s">
         <v>731</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>729</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>735</v>
+        <v>737</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>755</v>
+        <v>757</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>756</v>
+        <v>758</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>759</v>
+        <v>761</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>760</v>
+        <v>762</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>761</v>
+        <v>763</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>762</v>
+        <v>764</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>768</v>
+        <v>770</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>770</v>
+        <v>772</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>771</v>
+        <v>773</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>775</v>
+        <v>777</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
       <c r="B32" s="0" t="s">
+        <v>782</v>
+      </c>
+      <c r="C32" s="0" t="s">
         <v>780</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>778</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>786</v>
+        <v>788</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>787</v>
+        <v>789</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>788</v>
+        <v>790</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>790</v>
+        <v>792</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>792</v>
+        <v>794</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>793</v>
+        <v>795</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>794</v>
+        <v>796</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>801</v>
+        <v>803</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>808</v>
+        <v>810</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>813</v>
+        <v>815</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>817</v>
+        <v>819</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>818</v>
+        <v>820</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>819</v>
+        <v>821</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>820</v>
+        <v>822</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>825</v>
+        <v>827</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>826</v>
+        <v>828</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>828</v>
+        <v>830</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>830</v>
+        <v>832</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>834</v>
+        <v>836</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>835</v>
+        <v>837</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>838</v>
+        <v>840</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>838</v>
+        <v>840</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>840</v>
+        <v>842</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>842</v>
+        <v>844</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>843</v>
+        <v>845</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>845</v>
+        <v>847</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>846</v>
+        <v>848</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>847</v>
+        <v>849</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>848</v>
+        <v>850</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>849</v>
+        <v>851</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>850</v>
+        <v>852</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>851</v>
+        <v>853</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>852</v>
+        <v>854</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>853</v>
+        <v>855</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>854</v>
+        <v>856</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>855</v>
+        <v>857</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>856</v>
+        <v>858</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>857</v>
+        <v>859</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>858</v>
+        <v>860</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>859</v>
+        <v>861</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>860</v>
+        <v>862</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>861</v>
+        <v>863</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>862</v>
+        <v>864</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>863</v>
+        <v>865</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>864</v>
+        <v>866</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>868</v>
+        <v>870</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>869</v>
+        <v>871</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>870</v>
+        <v>872</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>871</v>
+        <v>873</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>872</v>
+        <v>874</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>873</v>
+        <v>875</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>874</v>
+        <v>876</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>875</v>
+        <v>877</v>
       </c>
       <c r="B65" s="0" t="s">
+        <v>878</v>
+      </c>
+      <c r="C65" s="0" t="s">
         <v>876</v>
-      </c>
-      <c r="C65" s="0" t="s">
-        <v>874</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>877</v>
+        <v>879</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>878</v>
+        <v>880</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>874</v>
+        <v>876</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>880</v>
+        <v>882</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>881</v>
+        <v>883</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>882</v>
+        <v>884</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>883</v>
+        <v>885</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>884</v>
+        <v>886</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>885</v>
+        <v>887</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>886</v>
+        <v>888</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>887</v>
+        <v>889</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>888</v>
+        <v>890</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>889</v>
+        <v>891</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>890</v>
+        <v>892</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>891</v>
+        <v>893</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>892</v>
+        <v>894</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>894</v>
+        <v>896</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>895</v>
+        <v>897</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>896</v>
+        <v>898</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>897</v>
+        <v>899</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>898</v>
+        <v>900</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>899</v>
+        <v>901</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>900</v>
+        <v>902</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>901</v>
+        <v>903</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>902</v>
+        <v>904</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>903</v>
+        <v>905</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>904</v>
+        <v>906</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>905</v>
+        <v>907</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>906</v>
+        <v>908</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>907</v>
+        <v>909</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>908</v>
+        <v>910</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>909</v>
+        <v>911</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>910</v>
+        <v>912</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>911</v>
+        <v>913</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>912</v>
+        <v>914</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>913</v>
+        <v>915</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>914</v>
+        <v>916</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>915</v>
+        <v>917</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[tests] update test suite
</commit_message>
<xml_diff>
--- a/web/fixtures/csv/test_data/carbure_template_advanced_missing_data_cannot_validate.xlsx
+++ b/web/fixtures/csv/test_data/carbure_template_advanced_missing_data_cannot_validate.xlsx
@@ -2905,10 +2905,10 @@
   <dimension ref="A1:AA3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.32"/>

</xml_diff>